<commit_message>
Adicionando Budesliga + BR
</commit_message>
<xml_diff>
--- a/de_para_siglas_bundesliga.xlsx
+++ b/de_para_siglas_bundesliga.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rafae\Google Drive\Projetos\SofaScore\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE96DA67-BBFC-4E57-8595-5932356DDB0A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A79D80D8-CB62-4265-A993-272AC13923CB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1560" yWindow="1560" windowWidth="15375" windowHeight="7875" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Planilha1!$A$1:$B$69</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Planilha1!$A$1:$B$70</definedName>
   </definedNames>
   <calcPr calcId="0" iterateDelta="1E-4"/>
   <extLst>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="109">
   <si>
     <t>time</t>
   </si>
@@ -352,6 +352,9 @@
   </si>
   <si>
     <t>Stuttgart</t>
+  </si>
+  <si>
+    <t>Darmstadt</t>
   </si>
 </sst>
 </file>
@@ -722,10 +725,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B87"/>
+  <dimension ref="A1:B88"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A50" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="B56" sqref="B56"/>
+    <sheetView tabSelected="1" topLeftCell="A53" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="B57" sqref="B57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1184,40 +1187,40 @@
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A57" s="5" t="s">
-        <v>62</v>
+      <c r="A57" s="6" t="s">
+        <v>108</v>
       </c>
       <c r="B57" s="6" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="B58" s="6" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A59" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="B58" s="6" t="s">
+      <c r="B59" s="6" t="s">
         <v>65</v>
-      </c>
-    </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A59" s="6" t="s">
-        <v>66</v>
-      </c>
-      <c r="B59" s="6" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A60" s="6" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B60" s="6" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A61" s="6" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B61" s="6" t="s">
         <v>69</v>
@@ -1225,7 +1228,7 @@
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A62" s="6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B62" s="6" t="s">
         <v>69</v>
@@ -1233,15 +1236,15 @@
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A63" s="6" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="B63" s="6" t="s">
-        <v>80</v>
+        <v>69</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A64" s="6" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B64" s="6" t="s">
         <v>80</v>
@@ -1249,84 +1252,92 @@
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A65" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="B65" s="6" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A66" s="6" t="s">
         <v>81</v>
       </c>
-      <c r="B65" s="6" t="s">
+      <c r="B66" s="6" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A66" s="4" t="s">
+    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A67" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="B66" s="6" t="s">
+      <c r="B67" s="6" t="s">
         <v>84</v>
-      </c>
-    </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A67" s="6" t="s">
-        <v>85</v>
-      </c>
-      <c r="B67" s="6" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A68" s="6" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B68" s="6" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A69" s="6" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B69" s="6" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A70" s="6" t="s">
-        <v>91</v>
-      </c>
-      <c r="B70" s="4" t="s">
-        <v>92</v>
+        <v>89</v>
+      </c>
+      <c r="B70" s="6" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A71" s="6" t="s">
-        <v>93</v>
-      </c>
-      <c r="B71" s="6" t="s">
-        <v>94</v>
+        <v>91</v>
+      </c>
+      <c r="B71" s="4" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A72" s="6" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B72" s="6" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A73" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="B73" s="6" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A74" s="6" t="s">
         <v>107</v>
       </c>
-      <c r="B73" s="6" t="s">
+      <c r="B74" s="6" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A86" s="3"/>
-    </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B87" s="2"/>
+      <c r="A87" s="3"/>
+    </row>
+    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B88" s="2"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:B69" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:B70" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <pageMargins left="0.51180555555555496" right="0.51180555555555496" top="0.78749999999999998" bottom="0.78749999999999998" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>

</xml_diff>